<commit_message>
Added 1 Flowchart & Semi-Final Feature List
</commit_message>
<xml_diff>
--- a/res/Feature Selection Sheet.xlsx
+++ b/res/Feature Selection Sheet.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9984" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9984" windowHeight="5928" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
   <si>
     <t>Search Corpus Creator: Q&amp;A Based Niched Searching</t>
   </si>
@@ -141,13 +142,73 @@
   </si>
   <si>
     <t>Reference Management Tool  ----&gt; DONE</t>
+  </si>
+  <si>
+    <t>Front-End Based Features</t>
+  </si>
+  <si>
+    <t>Back-End Based Features</t>
+  </si>
+  <si>
+    <t>Researcher's Dairy</t>
+  </si>
+  <si>
+    <t>External API Based Features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Keyword Corpus Creator </t>
+  </si>
+  <si>
+    <t>Providing Detailed Information Regarding - Funding Schemes</t>
+  </si>
+  <si>
+    <t>Research Platforms List [&amp; Cookie Based Checklist If Possible]</t>
+  </si>
+  <si>
+    <t>Ghost Writer - Hemingway Mode Writer</t>
+  </si>
+  <si>
+    <t>Research Process Management Tool - Task Assigning &amp; Tracking</t>
+  </si>
+  <si>
+    <t>Calender with Dates of Conferences [Not Through Web-Scrapper]</t>
+  </si>
+  <si>
+    <t>SMS &amp; Email Reminder Setter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Tips Provider </t>
+  </si>
+  <si>
+    <t>Chatbot for User Guide i.e. Troubleshooting FAQ of User while using the Platform</t>
+  </si>
+  <si>
+    <t>HTTPS &amp; JWT Based Security Based Web Application</t>
+  </si>
+  <si>
+    <t>Team Chat Feature</t>
+  </si>
+  <si>
+    <t>SME Paid Chat Feature</t>
+  </si>
+  <si>
+    <t>Thought Organiser Tools</t>
+  </si>
+  <si>
+    <t>Reference Management Tool</t>
+  </si>
+  <si>
+    <t>Plagiarism Checker [CopyLeak API or Other]</t>
+  </si>
+  <si>
+    <t>Grammer Checker [Ginger or Grammerly or Other]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +271,14 @@
     <font>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -280,7 +349,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -301,6 +370,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -589,8 +660,8 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G31" sqref="G11:H31"/>
+    <sheetView topLeftCell="A6" zoomScale="94" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -984,4 +1055,360 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="96" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:O44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B1:B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="72" customWidth="1"/>
+    <col min="13" max="15" width="47.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B1" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B3" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="15"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B6" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="3"/>
+      <c r="N8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="3"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B17" s="15"/>
+      <c r="M17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O17" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B18" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B19" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M19" s="11"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B20" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B21" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="M21" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M24" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M25" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M27" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M29" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="M32" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" spans="13:15" x14ac:dyDescent="0.3">
+      <c r="M33" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="13:15" x14ac:dyDescent="0.3">
+      <c r="M34" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+    </row>
+    <row r="35" spans="13:15" x14ac:dyDescent="0.3">
+      <c r="M35" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+    </row>
+    <row r="36" spans="13:15" x14ac:dyDescent="0.3">
+      <c r="M36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+    </row>
+    <row r="37" spans="13:15" x14ac:dyDescent="0.3">
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+    </row>
+    <row r="38" spans="13:15" x14ac:dyDescent="0.3">
+      <c r="M38" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="13:15" x14ac:dyDescent="0.3">
+      <c r="M39" s="7"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+    </row>
+    <row r="40" spans="13:15" x14ac:dyDescent="0.3">
+      <c r="M40" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+    </row>
+    <row r="41" spans="13:15" x14ac:dyDescent="0.3">
+      <c r="M41" s="7"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+    </row>
+    <row r="42" spans="13:15" x14ac:dyDescent="0.3">
+      <c r="M42" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+    </row>
+    <row r="43" spans="13:15" x14ac:dyDescent="0.3">
+      <c r="M43" s="7"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+    </row>
+    <row r="44" spans="13:15" x14ac:dyDescent="0.3">
+      <c r="M44" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>